<commit_message>
Add GitHub Action and release documentation
Introduces action.yml for M365 Security & Compliance Audit, usage examples, marketplace status, and release checklist for GitHub Actions Marketplace publication. Updates README with installation options and workflow patterns. Also adds XSS manual test, improves MCP server import, and updates devcontainer and VSCode settings for better development experience.
</commit_message>
<xml_diff>
--- a/output/reports/security/m365_cis_audit.xlsx
+++ b/output/reports/security/m365_cis_audit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Controls" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Overview" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Controls" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>